<commit_message>
JOBDESK ON PROGRESS 30/01/2019
</commit_message>
<xml_diff>
--- a/Report/Jobdesk.xlsx
+++ b/Report/Jobdesk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>achievement</t>
   </si>
@@ -89,33 +89,47 @@
     <t>iqbal</t>
   </si>
   <si>
-    <t>modul</t>
-  </si>
-  <si>
-    <t>nama</t>
-  </si>
-  <si>
-    <t>insert</t>
-  </si>
-  <si>
-    <t>update</t>
-  </si>
-  <si>
-    <t>delete</t>
-  </si>
-  <si>
-    <t>read</t>
-  </si>
-  <si>
-    <t>v</t>
+    <t>on progress</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>NAMA</t>
+  </si>
+  <si>
+    <t>MODUL</t>
+  </si>
+  <si>
+    <t>INSERT</t>
+  </si>
+  <si>
+    <t>READ</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>SEARCH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -131,7 +145,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -139,17 +153,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -434,36 +469,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>25</v>
+      <c r="E1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -474,12 +512,20 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -487,10 +533,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -499,10 +554,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -510,36 +574,66 @@
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -549,10 +643,19 @@
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -560,6 +663,11 @@
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -567,10 +675,19 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -579,10 +696,19 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -590,36 +716,66 @@
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -627,5 +783,6 @@
     <mergeCell ref="A11:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FIX insert, read, update, search
</commit_message>
<xml_diff>
--- a/Report/Jobdesk.xlsx
+++ b/Report/Jobdesk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
   <si>
     <t>achievement</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>SEARCH</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -172,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -185,6 +188,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -467,58 +473,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
+    <col min="4" max="7" width="12.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>21</v>
@@ -526,20 +532,23 @@
       <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>21</v>
@@ -547,20 +556,21 @@
       <c r="G3" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>21</v>
@@ -568,88 +578,99 @@
       <c r="G4" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>22</v>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>21</v>
@@ -657,31 +678,35 @@
       <c r="G11" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="H11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>22</v>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>21</v>
@@ -689,20 +714,23 @@
       <c r="G13" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>21</v>
@@ -710,72 +738,83 @@
       <c r="G14" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="H14" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="4"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Fix Database + Interfaces All
</commit_message>
<xml_diff>
--- a/Report/Jobdesk.xlsx
+++ b/Report/Jobdesk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="52">
   <si>
     <t>achievement</t>
   </si>
@@ -47,9 +47,6 @@
     <t>employee</t>
   </si>
   <si>
-    <t>erorbank</t>
-  </si>
-  <si>
     <t>historydetaillesson</t>
   </si>
   <si>
@@ -117,6 +114,72 @@
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>manage department</t>
+  </si>
+  <si>
+    <t>manage</t>
+  </si>
+  <si>
+    <t>manage placement</t>
+  </si>
+  <si>
+    <t>manage room</t>
+  </si>
+  <si>
+    <t>manage batch</t>
+  </si>
+  <si>
+    <t>manage class</t>
+  </si>
+  <si>
+    <t>Mentor</t>
+  </si>
+  <si>
+    <t>manage lesson</t>
+  </si>
+  <si>
+    <t>manage detaillesson</t>
+  </si>
+  <si>
+    <t>manage dailyscore</t>
+  </si>
+  <si>
+    <t>manage taskscore</t>
+  </si>
+  <si>
+    <t>manage schedule</t>
+  </si>
+  <si>
+    <t>manage student</t>
+  </si>
+  <si>
+    <t>manage employee</t>
+  </si>
+  <si>
+    <t>manage akun student</t>
+  </si>
+  <si>
+    <t>manage organization</t>
+  </si>
+  <si>
+    <t>manage achievement</t>
+  </si>
+  <si>
+    <t>manage skill</t>
+  </si>
+  <si>
+    <t>manage work experience</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>errorbank</t>
   </si>
 </sst>
 </file>
@@ -175,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -191,6 +254,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -473,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,100 +559,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>19</v>
+      <c r="A2" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -595,7 +644,7 @@
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -607,35 +656,57 @@
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="4"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
@@ -645,9 +716,9 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
@@ -657,35 +728,35 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>20</v>
+      <c r="A11" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
@@ -695,57 +766,45 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
@@ -755,23 +814,33 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
@@ -781,9 +850,9 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
@@ -793,9 +862,9 @@
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="2"/>
@@ -805,9 +874,9 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
@@ -816,10 +885,159 @@
       <c r="G20" s="2"/>
       <c r="H20" s="4"/>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+      <c r="C28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+      <c r="C31" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+      <c r="C33" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="A11:A20"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="B29:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>